<commit_message>
update thêm các cases vào workflow để gen ra các tình huống + update prompt để nó bá đạo : chống user lầy
</commit_message>
<xml_diff>
--- a/6_TuningWith2Prompting/src/CodeLogicCreateRoleUser/workflow_mece_table.xlsx
+++ b/6_TuningWith2Prompting/src/CodeLogicCreateRoleUser/workflow_mece_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/cuong_dn210141_sis_hust_edu_vn/Documents/GIT/BasicTasks_Prompting/6_TuningWith2Prompting/src/CodeLogicCreateRoleUser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A97DE6B-855C-47C1-B8D5-4D7BEF2FB336}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_F25DC773A252ABDACC104895C19E7EF25ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB27C5FF-12D3-4690-8F4F-680D388C920F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -45,52 +45,64 @@
     <t>user_intent_true</t>
   </si>
   <si>
-    <t>User trả lời câu 1 đúng</t>
-  </si>
-  <si>
     <t>user_intent_false</t>
   </si>
   <si>
-    <t>User trả lời câu 1 sai</t>
-  </si>
-  <si>
-    <t>User tiếp tục trả lời câu 1 sai</t>
-  </si>
-  <si>
     <t>PHỤ</t>
   </si>
   <si>
-    <t>User trả lời câu hỏi tiếp theo đúng.</t>
-  </si>
-  <si>
-    <t>User trả lời câu hỏi tiếp theo sai lần 1</t>
-  </si>
-  <si>
-    <t>User trả lời câu hỏi tiếp theo sai lần 2</t>
-  </si>
-  <si>
     <t>GỘP</t>
   </si>
   <si>
-    <t>User trả lời đúng khi được AI hỏi để gộp 2 câu hỏi ban đầu</t>
-  </si>
-  <si>
-    <t>User trả lời sai khi được AI hỏi để gộp 2 câu hỏi ban đầu</t>
-  </si>
-  <si>
-    <t>User tiếp tục trả lời sai khi được AI hỏi để gộp 2 câu hỏi ban đầu</t>
+    <t>1. Bạn sẽ trả lời câu 1 đúng</t>
+  </si>
+  <si>
+    <t>1. Bạn sẽ trả lời câu 1 sai: sai ngữ pháp.</t>
+  </si>
+  <si>
+    <t>1. Bạn sẽ trả lời câu 1 sai: sai intent.</t>
+  </si>
+  <si>
+    <t>1. Khi AI hỏi bạn câu 1, bạn sẽ trả lời sai 2 LẦN LIÊN TIẾP: 1 lần sai ngữ pháp, 1 lần sai intent.</t>
+  </si>
+  <si>
+    <t>2. Bạn sẽ trả lời câu hỏi tiếp theo đúng.</t>
+  </si>
+  <si>
+    <t>2. Bạn sẽ trả lời câu hỏi tiếp theo sai lần 1: sai ngữ pháp</t>
+  </si>
+  <si>
+    <t>2. Bạn sẽ trả lời câu hỏi tiếp theo sai lần 1: sai intent</t>
+  </si>
+  <si>
+    <t>2. Bạn sẽ trả lời câu hỏi tiếp theo sai 2 lần liên tiếp</t>
+  </si>
+  <si>
+    <t>3. Bạn sẽ trả lời đúng khi được AI hỏi để gộp 2 câu hỏi ban đầu</t>
+  </si>
+  <si>
+    <t>3. Khi được AI hỏi để gộp 2 câu hỏi ban đầu, bạn sẽ trả lời sai 1 lần: sai ngữ pháp</t>
+  </si>
+  <si>
+    <t>3. Khi được AI hỏi để gộp 2 câu hỏi ban đầu, bạn sẽ trả lời sai 1 lần: sai intent</t>
+  </si>
+  <si>
+    <t>3. Khi được AI hỏi để gộp 2 câu hỏi ban đầu, bạn sẽ trả lời sai 2 LẦN LIÊN TIẾP: 1 lần sai ngữ pháp, 1 lần sai intent</t>
   </si>
   <si>
     <t>HỎI LẠI</t>
   </si>
   <si>
-    <t>Khi được AI hỏi để trả lời lại cả câu =&gt; user trả lời đúng</t>
-  </si>
-  <si>
-    <t>Khi được AI hỏi để trả lời lại cả câu =&gt; user trả lời sai.</t>
-  </si>
-  <si>
-    <t>Khi được AI hỏi để trả lời lại cả câu =&gt; user tiếp tục trả lời sai.</t>
+    <t>4. Khi được AI hỏi để trả lời lại cả câu. Bạn sẽ trả lời đúng</t>
+  </si>
+  <si>
+    <t>4. Khi được AI hỏi để trả lời lại cả câu. Bạn sẽ trả lời sai 1 lần: sai ngữ pháp</t>
+  </si>
+  <si>
+    <t>4. Khi được AI hỏi để trả lời lại cả câu. Bạn sẽ trả lời sai 1 lần: sai intent</t>
+  </si>
+  <si>
+    <t>4. Khi được AI hỏi để trả lời lại cả câu. Bạn sẽ trả lời sai 2 lần liên tiếp: 1 lần sai ngữ pháp, 1 lần sai intent</t>
   </si>
 </sst>
 </file>
@@ -438,13 +450,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.109375" defaultRowHeight="30.6" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="51.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -471,7 +486,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -479,13 +494,13 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -493,66 +508,66 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>15</v>
@@ -560,13 +575,13 @@
     </row>
     <row r="9" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -574,13 +589,13 @@
     </row>
     <row r="10" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>17</v>
@@ -588,44 +603,100 @@
     </row>
     <row r="11" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2">
         <v>2</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D16" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>